<commit_message>
basic COCOMO effort estimation and basic Code Quality estimation has been implemented
</commit_message>
<xml_diff>
--- a/sheets/xlsxCouplings.xlsx
+++ b/sheets/xlsxCouplings.xlsx
@@ -459,21 +459,21 @@
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>MatchingEngine</v>
+        <v>IAaveDistributionManager</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>Morpho</v>
+        <v>IAaveIncentivesController</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -481,76 +481,76 @@
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>MorphoGovernance</v>
+        <v>IAToken</v>
       </c>
       <c r="B8">
         <v>2</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>MorphoStorage</v>
+        <v>IERC20</v>
       </c>
       <c r="B9">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C9">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>MorphoUtils</v>
+        <v>ILendingPool</v>
       </c>
       <c r="B10">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C10">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>PositionsManagerUtils</v>
+        <v>ILendingPoolAddressesProvider</v>
       </c>
       <c r="B11">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C11">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>IEntryPositionsManager</v>
+        <v>IPriceOracleGetter</v>
       </c>
       <c r="B12">
         <v>0</v>
       </c>
       <c r="C12">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>IExitPositionsManager</v>
+        <v>IScaledBalanceToken</v>
       </c>
       <c r="B13">
         <v>0</v>
       </c>
       <c r="C13">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>IGetterUnderlyingAsset</v>
+        <v>IVariableDebtToken</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -558,186 +558,186 @@
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>IIncentivesVault</v>
+        <v>IEntryPositionsManager</v>
       </c>
       <c r="B15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C15">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>IInterestRatesManager</v>
+        <v>IExitPositionsManager</v>
       </c>
       <c r="B16">
         <v>0</v>
       </c>
       <c r="C16">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>IMorpho</v>
+        <v>IGetterUnderlyingAsset</v>
       </c>
       <c r="B17">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C17">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>IOracle</v>
+        <v>IIncentivesVault</v>
       </c>
       <c r="B18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C18">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>IRewardsManager</v>
+        <v>IInterestRatesManager</v>
       </c>
       <c r="B19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C19">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>IAToken</v>
+        <v>IMorpho</v>
       </c>
       <c r="B20">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C20">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>IAaveDistributionManager</v>
+        <v>IOracle</v>
       </c>
       <c r="B21">
         <v>0</v>
       </c>
       <c r="C21">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="str">
-        <v>IAaveIncentivesController</v>
+        <v>IRewardsManager</v>
       </c>
       <c r="B22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C22">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v>IERC20</v>
+        <v>ILido</v>
       </c>
       <c r="B23">
         <v>0</v>
       </c>
       <c r="C23">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="str">
-        <v>ILendingPool</v>
+        <v>IndexesLens</v>
       </c>
       <c r="B24">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C24">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="str">
-        <v>ILendingPoolAddressesProvider</v>
+        <v>ILens</v>
       </c>
       <c r="B25">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C25">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="str">
-        <v>IPriceOracleGetter</v>
+        <v>Lens</v>
       </c>
       <c r="B26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C26">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="str">
-        <v>IScaledBalanceToken</v>
+        <v>LensStorage</v>
       </c>
       <c r="B27">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="C27">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="str">
-        <v>IVariableDebtToken</v>
+        <v>MarketsLens</v>
       </c>
       <c r="B28">
         <v>1</v>
       </c>
       <c r="C28">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="str">
-        <v>ILido</v>
+        <v>RatesLens</v>
       </c>
       <c r="B29">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C29">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="str">
-        <v>IndexesLens</v>
+        <v>UsersLens</v>
       </c>
       <c r="B30">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C30">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="str">
-        <v>Lens</v>
+        <v>DataTypes</v>
       </c>
       <c r="B31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C31">
         <v>0</v>
@@ -745,123 +745,123 @@
     </row>
     <row r="32">
       <c r="A32" t="str">
-        <v>LensStorage</v>
+        <v>Errors</v>
       </c>
       <c r="B32">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="C32">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="str">
-        <v>MarketsLens</v>
+        <v>ReserveConfiguration</v>
       </c>
       <c r="B33">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C33">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="str">
-        <v>RatesLens</v>
+        <v>UserConfiguration</v>
       </c>
       <c r="B34">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C34">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="str">
-        <v>UsersLens</v>
+        <v>InterestRatesModel</v>
       </c>
       <c r="B35">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C35">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="str">
-        <v>ILens</v>
+        <v>Types</v>
       </c>
       <c r="B36">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C36">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="str">
-        <v>InterestRatesModel</v>
+        <v>MatchingEngine</v>
       </c>
       <c r="B37">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C37">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="str">
-        <v>Types</v>
+        <v>Morpho</v>
       </c>
       <c r="B38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C38">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="str">
-        <v>DataTypes</v>
+        <v>MorphoGovernance</v>
       </c>
       <c r="B39">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C39">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="str">
-        <v>Errors</v>
+        <v>MorphoStorage</v>
       </c>
       <c r="B40">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C40">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="str">
-        <v>ReserveConfiguration</v>
+        <v>MorphoUtils</v>
       </c>
       <c r="B41">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="C41">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="str">
-        <v>UserConfiguration</v>
+        <v>PositionsManagerUtils</v>
       </c>
       <c r="B42">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C42">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43">
@@ -910,21 +910,21 @@
     </row>
     <row r="47">
       <c r="A47" t="str">
-        <v>MatchingEngine</v>
+        <v>ICEth</v>
       </c>
       <c r="B47">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C47">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="str">
-        <v>Morpho</v>
+        <v>IComptroller</v>
       </c>
       <c r="B48">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C48">
         <v>0</v>
@@ -932,43 +932,43 @@
     </row>
     <row r="49">
       <c r="A49" t="str">
-        <v>MorphoGovernance</v>
+        <v>IInterestRateModel</v>
       </c>
       <c r="B49">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C49">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="str">
-        <v>MorphoStorage</v>
+        <v>ICToken</v>
       </c>
       <c r="B50">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="C50">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="str">
-        <v>MorphoUtils</v>
+        <v>ICEther</v>
       </c>
       <c r="B51">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C51">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="str">
-        <v>PositionsManager</v>
+        <v>ICompoundOracle</v>
       </c>
       <c r="B52">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C52">
         <v>0</v>
@@ -976,10 +976,10 @@
     </row>
     <row r="53">
       <c r="A53" t="str">
-        <v>RewardsManager</v>
+        <v>IIncentivesVault</v>
       </c>
       <c r="B53">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C53">
         <v>0</v>
@@ -987,164 +987,164 @@
     </row>
     <row r="54">
       <c r="A54" t="str">
-        <v>IIncentivesVault</v>
+        <v>IInterestRatesManager</v>
       </c>
       <c r="B54">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C54">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="str">
-        <v>IInterestRatesManager</v>
+        <v>IMorpho</v>
       </c>
       <c r="B55">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C55">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="str">
-        <v>IMorpho</v>
+        <v>IOracle</v>
       </c>
       <c r="B56">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C56">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="str">
-        <v>IOracle</v>
+        <v>IPositionsManager</v>
       </c>
       <c r="B57">
         <v>0</v>
       </c>
       <c r="C57">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="str">
-        <v>IPositionsManager</v>
+        <v>IRewardsManager</v>
       </c>
       <c r="B58">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C58">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="str">
-        <v>IRewardsManager</v>
+        <v>IWETH</v>
       </c>
       <c r="B59">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C59">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="str">
-        <v>IWETH</v>
+        <v>IndexesLens</v>
       </c>
       <c r="B60">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C60">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="str">
-        <v>ICEth</v>
+        <v>ILens</v>
       </c>
       <c r="B61">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C61">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="str">
-        <v>IComptroller</v>
+        <v>Lens</v>
       </c>
       <c r="B62">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C62">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="str">
-        <v>IInterestRateModel</v>
+        <v>LensStorage</v>
       </c>
       <c r="B63">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="C63">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="str">
-        <v>ICToken</v>
+        <v>MarketsLens</v>
       </c>
       <c r="B64">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C64">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="str">
-        <v>ICEther</v>
+        <v>RatesLens</v>
       </c>
       <c r="B65">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C65">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="str">
-        <v>ICompoundOracle</v>
+        <v>RewardsLens</v>
       </c>
       <c r="B66">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C66">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="str">
-        <v>IndexesLens</v>
+        <v>UsersLens</v>
       </c>
       <c r="B67">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C67">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="str">
-        <v>Lens</v>
+        <v>CompoundMath</v>
       </c>
       <c r="B68">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C68">
         <v>0</v>
@@ -1152,101 +1152,101 @@
     </row>
     <row r="69">
       <c r="A69" t="str">
-        <v>LensStorage</v>
+        <v>InterestRatesModel</v>
       </c>
       <c r="B69">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C69">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="str">
-        <v>MarketsLens</v>
+        <v>Types</v>
       </c>
       <c r="B70">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C70">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="str">
-        <v>RatesLens</v>
+        <v>MatchingEngine</v>
       </c>
       <c r="B71">
         <v>1</v>
       </c>
       <c r="C71">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="str">
-        <v>RewardsLens</v>
+        <v>Morpho</v>
       </c>
       <c r="B72">
         <v>1</v>
       </c>
       <c r="C72">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="str">
-        <v>UsersLens</v>
+        <v>MorphoGovernance</v>
       </c>
       <c r="B73">
         <v>1</v>
       </c>
       <c r="C73">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="str">
-        <v>ILens</v>
+        <v>MorphoStorage</v>
       </c>
       <c r="B74">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C74">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="str">
-        <v>CompoundMath</v>
+        <v>MorphoUtils</v>
       </c>
       <c r="B75">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C75">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="str">
-        <v>InterestRatesModel</v>
+        <v>PositionsManager</v>
       </c>
       <c r="B76">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C76">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="str">
-        <v>Types</v>
+        <v>RewardsManager</v>
       </c>
       <c r="B77">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C77">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
another example project added for demonstration
</commit_message>
<xml_diff>
--- a/sheets/xlsxCouplings.xlsx
+++ b/sheets/xlsxCouplings.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C77"/>
+  <dimension ref="A1:C63"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -415,10 +415,10 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>EntryPositionsManager</v>
+        <v>IUniswapV3FlashCallback</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -426,10 +426,10 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>ExitPositionsManager</v>
+        <v>IUniswapV3MintCallback</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -437,10 +437,10 @@
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>IncentivesVault</v>
+        <v>IUniswapV3SwapCallback</v>
       </c>
       <c r="B4">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -448,10 +448,10 @@
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>InterestRatesManager</v>
+        <v>IERC20Minimal</v>
       </c>
       <c r="B5">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -459,7 +459,7 @@
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>IAaveDistributionManager</v>
+        <v>IUniswapV3Factory</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -470,10 +470,10 @@
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>IAaveIncentivesController</v>
+        <v>IUniswapV3Pool</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -481,10 +481,10 @@
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>IAToken</v>
+        <v>IUniswapV3PoolDeployer</v>
       </c>
       <c r="B8">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -492,7 +492,7 @@
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>IERC20</v>
+        <v>IUniswapV3PoolActions</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -503,10 +503,10 @@
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>ILendingPool</v>
+        <v>IUniswapV3PoolDerivedState</v>
       </c>
       <c r="B10">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -514,7 +514,7 @@
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>ILendingPoolAddressesProvider</v>
+        <v>IUniswapV3PoolEvents</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -525,7 +525,7 @@
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>IPriceOracleGetter</v>
+        <v>IUniswapV3PoolImmutables</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -536,7 +536,7 @@
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>IScaledBalanceToken</v>
+        <v>IUniswapV3PoolOwnerActions</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -547,10 +547,10 @@
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>IVariableDebtToken</v>
+        <v>IUniswapV3PoolState</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -558,7 +558,7 @@
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>IEntryPositionsManager</v>
+        <v>BitMath</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -569,7 +569,7 @@
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>IExitPositionsManager</v>
+        <v>FixedPoint128</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -580,7 +580,7 @@
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>IGetterUnderlyingAsset</v>
+        <v>FixedPoint96</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -591,10 +591,10 @@
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>IIncentivesVault</v>
+        <v>FullMath</v>
       </c>
       <c r="B18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -602,7 +602,7 @@
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>IInterestRatesManager</v>
+        <v>LiquidityMath</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -613,10 +613,10 @@
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>IMorpho</v>
+        <v>LowGasSafeMath</v>
       </c>
       <c r="B20">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C20">
         <v>0</v>
@@ -624,7 +624,7 @@
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>IOracle</v>
+        <v>Oracle</v>
       </c>
       <c r="B21">
         <v>0</v>
@@ -635,10 +635,10 @@
     </row>
     <row r="22">
       <c r="A22" t="str">
-        <v>IRewardsManager</v>
+        <v>Position</v>
       </c>
       <c r="B22">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C22">
         <v>0</v>
@@ -646,7 +646,7 @@
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v>ILido</v>
+        <v>SafeCast</v>
       </c>
       <c r="B23">
         <v>0</v>
@@ -657,10 +657,10 @@
     </row>
     <row r="24">
       <c r="A24" t="str">
-        <v>IndexesLens</v>
+        <v>SqrtPriceMath</v>
       </c>
       <c r="B24">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C24">
         <v>0</v>
@@ -668,10 +668,10 @@
     </row>
     <row r="25">
       <c r="A25" t="str">
-        <v>ILens</v>
+        <v>SwapMath</v>
       </c>
       <c r="B25">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C25">
         <v>0</v>
@@ -679,10 +679,10 @@
     </row>
     <row r="26">
       <c r="A26" t="str">
-        <v>Lens</v>
+        <v>Tick</v>
       </c>
       <c r="B26">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C26">
         <v>0</v>
@@ -690,10 +690,10 @@
     </row>
     <row r="27">
       <c r="A27" t="str">
-        <v>LensStorage</v>
+        <v>TickBitmap</v>
       </c>
       <c r="B27">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="C27">
         <v>0</v>
@@ -701,10 +701,10 @@
     </row>
     <row r="28">
       <c r="A28" t="str">
-        <v>MarketsLens</v>
+        <v>TickMath</v>
       </c>
       <c r="B28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C28">
         <v>0</v>
@@ -712,10 +712,10 @@
     </row>
     <row r="29">
       <c r="A29" t="str">
-        <v>RatesLens</v>
+        <v>TransferHelper</v>
       </c>
       <c r="B29">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C29">
         <v>0</v>
@@ -723,10 +723,10 @@
     </row>
     <row r="30">
       <c r="A30" t="str">
-        <v>UsersLens</v>
+        <v>UnsafeMath</v>
       </c>
       <c r="B30">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C30">
         <v>0</v>
@@ -734,7 +734,7 @@
     </row>
     <row r="31">
       <c r="A31" t="str">
-        <v>DataTypes</v>
+        <v>NoDelegateCall</v>
       </c>
       <c r="B31">
         <v>0</v>
@@ -745,10 +745,10 @@
     </row>
     <row r="32">
       <c r="A32" t="str">
-        <v>Errors</v>
+        <v>BitMathEchidnaTest</v>
       </c>
       <c r="B32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C32">
         <v>0</v>
@@ -756,10 +756,10 @@
     </row>
     <row r="33">
       <c r="A33" t="str">
-        <v>ReserveConfiguration</v>
+        <v>BitMathTest</v>
       </c>
       <c r="B33">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C33">
         <v>0</v>
@@ -767,7 +767,7 @@
     </row>
     <row r="34">
       <c r="A34" t="str">
-        <v>UserConfiguration</v>
+        <v>FullMathEchidnaTest</v>
       </c>
       <c r="B34">
         <v>1</v>
@@ -778,10 +778,10 @@
     </row>
     <row r="35">
       <c r="A35" t="str">
-        <v>InterestRatesModel</v>
+        <v>FullMathTest</v>
       </c>
       <c r="B35">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C35">
         <v>0</v>
@@ -789,10 +789,10 @@
     </row>
     <row r="36">
       <c r="A36" t="str">
-        <v>Types</v>
+        <v>LiquidityMathTest</v>
       </c>
       <c r="B36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C36">
         <v>0</v>
@@ -800,7 +800,7 @@
     </row>
     <row r="37">
       <c r="A37" t="str">
-        <v>MatchingEngine</v>
+        <v>LowGasSafeMathEchidnaTest</v>
       </c>
       <c r="B37">
         <v>1</v>
@@ -811,7 +811,7 @@
     </row>
     <row r="38">
       <c r="A38" t="str">
-        <v>Morpho</v>
+        <v>MockTimeUniswapV3Pool</v>
       </c>
       <c r="B38">
         <v>1</v>
@@ -822,7 +822,7 @@
     </row>
     <row r="39">
       <c r="A39" t="str">
-        <v>MorphoGovernance</v>
+        <v>MockTimeUniswapV3PoolDeployer</v>
       </c>
       <c r="B39">
         <v>2</v>
@@ -833,10 +833,10 @@
     </row>
     <row r="40">
       <c r="A40" t="str">
-        <v>MorphoStorage</v>
+        <v>NoDelegateCallTest</v>
       </c>
       <c r="B40">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C40">
         <v>0</v>
@@ -844,10 +844,10 @@
     </row>
     <row r="41">
       <c r="A41" t="str">
-        <v>MorphoUtils</v>
+        <v>OracleEchidnaTest</v>
       </c>
       <c r="B41">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C41">
         <v>0</v>
@@ -855,10 +855,10 @@
     </row>
     <row r="42">
       <c r="A42" t="str">
-        <v>PositionsManagerUtils</v>
+        <v>OracleTest</v>
       </c>
       <c r="B42">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C42">
         <v>0</v>
@@ -866,7 +866,7 @@
     </row>
     <row r="43">
       <c r="A43" t="str">
-        <v>RewardsDistributor</v>
+        <v>SqrtPriceMathEchidnaTest</v>
       </c>
       <c r="B43">
         <v>3</v>
@@ -877,7 +877,7 @@
     </row>
     <row r="44">
       <c r="A44" t="str">
-        <v>FakeToken</v>
+        <v>SqrtPriceMathTest</v>
       </c>
       <c r="B44">
         <v>1</v>
@@ -888,10 +888,10 @@
     </row>
     <row r="45">
       <c r="A45" t="str">
-        <v>IncentivesVault</v>
+        <v>SwapMathEchidnaTest</v>
       </c>
       <c r="B45">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C45">
         <v>0</v>
@@ -899,10 +899,10 @@
     </row>
     <row r="46">
       <c r="A46" t="str">
-        <v>InterestRatesManager</v>
+        <v>SwapMathTest</v>
       </c>
       <c r="B46">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C46">
         <v>0</v>
@@ -910,10 +910,10 @@
     </row>
     <row r="47">
       <c r="A47" t="str">
-        <v>ICEth</v>
+        <v>TestERC20</v>
       </c>
       <c r="B47">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C47">
         <v>0</v>
@@ -921,10 +921,10 @@
     </row>
     <row r="48">
       <c r="A48" t="str">
-        <v>IComptroller</v>
+        <v>TestUniswapV3Callee</v>
       </c>
       <c r="B48">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="C48">
         <v>0</v>
@@ -932,10 +932,10 @@
     </row>
     <row r="49">
       <c r="A49" t="str">
-        <v>IInterestRateModel</v>
+        <v>TestUniswapV3ReentrantCallee</v>
       </c>
       <c r="B49">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C49">
         <v>0</v>
@@ -943,10 +943,10 @@
     </row>
     <row r="50">
       <c r="A50" t="str">
-        <v>ICToken</v>
+        <v>TestUniswapV3Router</v>
       </c>
       <c r="B50">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C50">
         <v>0</v>
@@ -954,10 +954,10 @@
     </row>
     <row r="51">
       <c r="A51" t="str">
-        <v>ICEther</v>
+        <v>TestUniswapV3SwapPay</v>
       </c>
       <c r="B51">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C51">
         <v>0</v>
@@ -965,10 +965,10 @@
     </row>
     <row r="52">
       <c r="A52" t="str">
-        <v>ICompoundOracle</v>
+        <v>TickBitmapEchidnaTest</v>
       </c>
       <c r="B52">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C52">
         <v>0</v>
@@ -976,7 +976,7 @@
     </row>
     <row r="53">
       <c r="A53" t="str">
-        <v>IIncentivesVault</v>
+        <v>TickBitmapTest</v>
       </c>
       <c r="B53">
         <v>1</v>
@@ -987,10 +987,10 @@
     </row>
     <row r="54">
       <c r="A54" t="str">
-        <v>IInterestRatesManager</v>
+        <v>TickEchidnaTest</v>
       </c>
       <c r="B54">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C54">
         <v>0</v>
@@ -998,10 +998,10 @@
     </row>
     <row r="55">
       <c r="A55" t="str">
-        <v>IMorpho</v>
+        <v>TickMathEchidnaTest</v>
       </c>
       <c r="B55">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C55">
         <v>0</v>
@@ -1009,10 +1009,10 @@
     </row>
     <row r="56">
       <c r="A56" t="str">
-        <v>IOracle</v>
+        <v>TickMathTest</v>
       </c>
       <c r="B56">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C56">
         <v>0</v>
@@ -1020,10 +1020,10 @@
     </row>
     <row r="57">
       <c r="A57" t="str">
-        <v>IPositionsManager</v>
+        <v>TickOverflowSafetyEchidnaTest</v>
       </c>
       <c r="B57">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C57">
         <v>0</v>
@@ -1031,7 +1031,7 @@
     </row>
     <row r="58">
       <c r="A58" t="str">
-        <v>IRewardsManager</v>
+        <v>TickTest</v>
       </c>
       <c r="B58">
         <v>1</v>
@@ -1042,10 +1042,10 @@
     </row>
     <row r="59">
       <c r="A59" t="str">
-        <v>IWETH</v>
+        <v>UniswapV3PoolSwapTest</v>
       </c>
       <c r="B59">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C59">
         <v>0</v>
@@ -1053,10 +1053,10 @@
     </row>
     <row r="60">
       <c r="A60" t="str">
-        <v>IndexesLens</v>
+        <v>UnsafeMathEchidnaTest</v>
       </c>
       <c r="B60">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C60">
         <v>0</v>
@@ -1064,10 +1064,10 @@
     </row>
     <row r="61">
       <c r="A61" t="str">
-        <v>ILens</v>
+        <v>UniswapV3Factory</v>
       </c>
       <c r="B61">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C61">
         <v>0</v>
@@ -1075,10 +1075,10 @@
     </row>
     <row r="62">
       <c r="A62" t="str">
-        <v>Lens</v>
+        <v>UniswapV3Pool</v>
       </c>
       <c r="B62">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="C62">
         <v>0</v>
@@ -1086,172 +1086,18 @@
     </row>
     <row r="63">
       <c r="A63" t="str">
-        <v>LensStorage</v>
+        <v>UniswapV3PoolDeployer</v>
       </c>
       <c r="B63">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C63">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" t="str">
-        <v>MarketsLens</v>
-      </c>
-      <c r="B64">
-        <v>1</v>
-      </c>
-      <c r="C64">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" t="str">
-        <v>RatesLens</v>
-      </c>
-      <c r="B65">
-        <v>1</v>
-      </c>
-      <c r="C65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" t="str">
-        <v>RewardsLens</v>
-      </c>
-      <c r="B66">
-        <v>1</v>
-      </c>
-      <c r="C66">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" t="str">
-        <v>UsersLens</v>
-      </c>
-      <c r="B67">
-        <v>1</v>
-      </c>
-      <c r="C67">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" t="str">
-        <v>CompoundMath</v>
-      </c>
-      <c r="B68">
-        <v>0</v>
-      </c>
-      <c r="C68">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" t="str">
-        <v>InterestRatesModel</v>
-      </c>
-      <c r="B69">
-        <v>4</v>
-      </c>
-      <c r="C69">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" t="str">
-        <v>Types</v>
-      </c>
-      <c r="B70">
-        <v>0</v>
-      </c>
-      <c r="C70">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" t="str">
-        <v>MatchingEngine</v>
-      </c>
-      <c r="B71">
-        <v>1</v>
-      </c>
-      <c r="C71">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" t="str">
-        <v>Morpho</v>
-      </c>
-      <c r="B72">
-        <v>1</v>
-      </c>
-      <c r="C72">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" t="str">
-        <v>MorphoGovernance</v>
-      </c>
-      <c r="B73">
-        <v>1</v>
-      </c>
-      <c r="C73">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" t="str">
-        <v>MorphoStorage</v>
-      </c>
-      <c r="B74">
-        <v>9</v>
-      </c>
-      <c r="C74">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" t="str">
-        <v>MorphoUtils</v>
-      </c>
-      <c r="B75">
-        <v>5</v>
-      </c>
-      <c r="C75">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" t="str">
-        <v>PositionsManager</v>
-      </c>
-      <c r="B76">
-        <v>3</v>
-      </c>
-      <c r="C76">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" t="str">
-        <v>RewardsManager</v>
-      </c>
-      <c r="B77">
-        <v>4</v>
-      </c>
-      <c r="C77">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C77"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C63"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
error in the contract complexity weights has been fixed
</commit_message>
<xml_diff>
--- a/sheets/xlsxCouplings.xlsx
+++ b/sheets/xlsxCouplings.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C63"/>
+  <dimension ref="A1:C77"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -415,10 +415,10 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>IUniswapV3FlashCallback</v>
+        <v>EntryPositionsManager</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -426,10 +426,10 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>IUniswapV3MintCallback</v>
+        <v>ExitPositionsManager</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -437,10 +437,10 @@
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>IUniswapV3SwapCallback</v>
+        <v>IncentivesVault</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -448,10 +448,10 @@
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>IERC20Minimal</v>
+        <v>InterestRatesManager</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -459,7 +459,7 @@
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>IUniswapV3Factory</v>
+        <v>IAaveDistributionManager</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -470,10 +470,10 @@
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>IUniswapV3Pool</v>
+        <v>IAaveIncentivesController</v>
       </c>
       <c r="B7">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -481,10 +481,10 @@
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>IUniswapV3PoolDeployer</v>
+        <v>IAToken</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -492,7 +492,7 @@
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>IUniswapV3PoolActions</v>
+        <v>IERC20</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -503,10 +503,10 @@
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>IUniswapV3PoolDerivedState</v>
+        <v>ILendingPool</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -514,7 +514,7 @@
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>IUniswapV3PoolEvents</v>
+        <v>ILendingPoolAddressesProvider</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -525,7 +525,7 @@
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>IUniswapV3PoolImmutables</v>
+        <v>IPriceOracleGetter</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -536,7 +536,7 @@
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>IUniswapV3PoolOwnerActions</v>
+        <v>IScaledBalanceToken</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -547,10 +547,10 @@
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>IUniswapV3PoolState</v>
+        <v>IVariableDebtToken</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -558,7 +558,7 @@
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>BitMath</v>
+        <v>IEntryPositionsManager</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -569,7 +569,7 @@
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>FixedPoint128</v>
+        <v>IExitPositionsManager</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -580,7 +580,7 @@
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>FixedPoint96</v>
+        <v>IGetterUnderlyingAsset</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -591,10 +591,10 @@
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>FullMath</v>
+        <v>IIncentivesVault</v>
       </c>
       <c r="B18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -602,7 +602,7 @@
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>LiquidityMath</v>
+        <v>IInterestRatesManager</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -613,10 +613,10 @@
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>LowGasSafeMath</v>
+        <v>IMorpho</v>
       </c>
       <c r="B20">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C20">
         <v>0</v>
@@ -624,7 +624,7 @@
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>Oracle</v>
+        <v>IOracle</v>
       </c>
       <c r="B21">
         <v>0</v>
@@ -635,10 +635,10 @@
     </row>
     <row r="22">
       <c r="A22" t="str">
-        <v>Position</v>
+        <v>IRewardsManager</v>
       </c>
       <c r="B22">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C22">
         <v>0</v>
@@ -646,7 +646,7 @@
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v>SafeCast</v>
+        <v>ILido</v>
       </c>
       <c r="B23">
         <v>0</v>
@@ -657,10 +657,10 @@
     </row>
     <row r="24">
       <c r="A24" t="str">
-        <v>SqrtPriceMath</v>
+        <v>IndexesLens</v>
       </c>
       <c r="B24">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C24">
         <v>0</v>
@@ -668,10 +668,10 @@
     </row>
     <row r="25">
       <c r="A25" t="str">
-        <v>SwapMath</v>
+        <v>ILens</v>
       </c>
       <c r="B25">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C25">
         <v>0</v>
@@ -679,10 +679,10 @@
     </row>
     <row r="26">
       <c r="A26" t="str">
-        <v>Tick</v>
+        <v>Lens</v>
       </c>
       <c r="B26">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C26">
         <v>0</v>
@@ -690,10 +690,10 @@
     </row>
     <row r="27">
       <c r="A27" t="str">
-        <v>TickBitmap</v>
+        <v>LensStorage</v>
       </c>
       <c r="B27">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C27">
         <v>0</v>
@@ -701,10 +701,10 @@
     </row>
     <row r="28">
       <c r="A28" t="str">
-        <v>TickMath</v>
+        <v>MarketsLens</v>
       </c>
       <c r="B28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C28">
         <v>0</v>
@@ -712,10 +712,10 @@
     </row>
     <row r="29">
       <c r="A29" t="str">
-        <v>TransferHelper</v>
+        <v>RatesLens</v>
       </c>
       <c r="B29">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C29">
         <v>0</v>
@@ -723,10 +723,10 @@
     </row>
     <row r="30">
       <c r="A30" t="str">
-        <v>UnsafeMath</v>
+        <v>UsersLens</v>
       </c>
       <c r="B30">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C30">
         <v>0</v>
@@ -734,7 +734,7 @@
     </row>
     <row r="31">
       <c r="A31" t="str">
-        <v>NoDelegateCall</v>
+        <v>DataTypes</v>
       </c>
       <c r="B31">
         <v>0</v>
@@ -745,10 +745,10 @@
     </row>
     <row r="32">
       <c r="A32" t="str">
-        <v>BitMathEchidnaTest</v>
+        <v>Errors</v>
       </c>
       <c r="B32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C32">
         <v>0</v>
@@ -756,10 +756,10 @@
     </row>
     <row r="33">
       <c r="A33" t="str">
-        <v>BitMathTest</v>
+        <v>ReserveConfiguration</v>
       </c>
       <c r="B33">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C33">
         <v>0</v>
@@ -767,7 +767,7 @@
     </row>
     <row r="34">
       <c r="A34" t="str">
-        <v>FullMathEchidnaTest</v>
+        <v>UserConfiguration</v>
       </c>
       <c r="B34">
         <v>1</v>
@@ -778,10 +778,10 @@
     </row>
     <row r="35">
       <c r="A35" t="str">
-        <v>FullMathTest</v>
+        <v>InterestRatesModel</v>
       </c>
       <c r="B35">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C35">
         <v>0</v>
@@ -789,10 +789,10 @@
     </row>
     <row r="36">
       <c r="A36" t="str">
-        <v>LiquidityMathTest</v>
+        <v>Types</v>
       </c>
       <c r="B36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C36">
         <v>0</v>
@@ -800,7 +800,7 @@
     </row>
     <row r="37">
       <c r="A37" t="str">
-        <v>LowGasSafeMathEchidnaTest</v>
+        <v>MatchingEngine</v>
       </c>
       <c r="B37">
         <v>1</v>
@@ -811,7 +811,7 @@
     </row>
     <row r="38">
       <c r="A38" t="str">
-        <v>MockTimeUniswapV3Pool</v>
+        <v>Morpho</v>
       </c>
       <c r="B38">
         <v>1</v>
@@ -822,7 +822,7 @@
     </row>
     <row r="39">
       <c r="A39" t="str">
-        <v>MockTimeUniswapV3PoolDeployer</v>
+        <v>MorphoGovernance</v>
       </c>
       <c r="B39">
         <v>2</v>
@@ -833,10 +833,10 @@
     </row>
     <row r="40">
       <c r="A40" t="str">
-        <v>NoDelegateCallTest</v>
+        <v>MorphoStorage</v>
       </c>
       <c r="B40">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C40">
         <v>0</v>
@@ -844,10 +844,10 @@
     </row>
     <row r="41">
       <c r="A41" t="str">
-        <v>OracleEchidnaTest</v>
+        <v>MorphoUtils</v>
       </c>
       <c r="B41">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C41">
         <v>0</v>
@@ -855,10 +855,10 @@
     </row>
     <row r="42">
       <c r="A42" t="str">
-        <v>OracleTest</v>
+        <v>PositionsManagerUtils</v>
       </c>
       <c r="B42">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C42">
         <v>0</v>
@@ -866,7 +866,7 @@
     </row>
     <row r="43">
       <c r="A43" t="str">
-        <v>SqrtPriceMathEchidnaTest</v>
+        <v>RewardsDistributor</v>
       </c>
       <c r="B43">
         <v>3</v>
@@ -877,7 +877,7 @@
     </row>
     <row r="44">
       <c r="A44" t="str">
-        <v>SqrtPriceMathTest</v>
+        <v>FakeToken</v>
       </c>
       <c r="B44">
         <v>1</v>
@@ -888,10 +888,10 @@
     </row>
     <row r="45">
       <c r="A45" t="str">
-        <v>SwapMathEchidnaTest</v>
+        <v>IncentivesVault</v>
       </c>
       <c r="B45">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C45">
         <v>0</v>
@@ -899,10 +899,10 @@
     </row>
     <row r="46">
       <c r="A46" t="str">
-        <v>SwapMathTest</v>
+        <v>InterestRatesManager</v>
       </c>
       <c r="B46">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C46">
         <v>0</v>
@@ -910,10 +910,10 @@
     </row>
     <row r="47">
       <c r="A47" t="str">
-        <v>TestERC20</v>
+        <v>ICEth</v>
       </c>
       <c r="B47">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C47">
         <v>0</v>
@@ -921,10 +921,10 @@
     </row>
     <row r="48">
       <c r="A48" t="str">
-        <v>TestUniswapV3Callee</v>
+        <v>IComptroller</v>
       </c>
       <c r="B48">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="C48">
         <v>0</v>
@@ -932,10 +932,10 @@
     </row>
     <row r="49">
       <c r="A49" t="str">
-        <v>TestUniswapV3ReentrantCallee</v>
+        <v>IInterestRateModel</v>
       </c>
       <c r="B49">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C49">
         <v>0</v>
@@ -943,10 +943,10 @@
     </row>
     <row r="50">
       <c r="A50" t="str">
-        <v>TestUniswapV3Router</v>
+        <v>ICToken</v>
       </c>
       <c r="B50">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C50">
         <v>0</v>
@@ -954,10 +954,10 @@
     </row>
     <row r="51">
       <c r="A51" t="str">
-        <v>TestUniswapV3SwapPay</v>
+        <v>ICEther</v>
       </c>
       <c r="B51">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C51">
         <v>0</v>
@@ -965,10 +965,10 @@
     </row>
     <row r="52">
       <c r="A52" t="str">
-        <v>TickBitmapEchidnaTest</v>
+        <v>ICompoundOracle</v>
       </c>
       <c r="B52">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C52">
         <v>0</v>
@@ -976,7 +976,7 @@
     </row>
     <row r="53">
       <c r="A53" t="str">
-        <v>TickBitmapTest</v>
+        <v>IIncentivesVault</v>
       </c>
       <c r="B53">
         <v>1</v>
@@ -987,10 +987,10 @@
     </row>
     <row r="54">
       <c r="A54" t="str">
-        <v>TickEchidnaTest</v>
+        <v>IInterestRatesManager</v>
       </c>
       <c r="B54">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C54">
         <v>0</v>
@@ -998,10 +998,10 @@
     </row>
     <row r="55">
       <c r="A55" t="str">
-        <v>TickMathEchidnaTest</v>
+        <v>IMorpho</v>
       </c>
       <c r="B55">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C55">
         <v>0</v>
@@ -1009,10 +1009,10 @@
     </row>
     <row r="56">
       <c r="A56" t="str">
-        <v>TickMathTest</v>
+        <v>IOracle</v>
       </c>
       <c r="B56">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C56">
         <v>0</v>
@@ -1020,10 +1020,10 @@
     </row>
     <row r="57">
       <c r="A57" t="str">
-        <v>TickOverflowSafetyEchidnaTest</v>
+        <v>IPositionsManager</v>
       </c>
       <c r="B57">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C57">
         <v>0</v>
@@ -1031,7 +1031,7 @@
     </row>
     <row r="58">
       <c r="A58" t="str">
-        <v>TickTest</v>
+        <v>IRewardsManager</v>
       </c>
       <c r="B58">
         <v>1</v>
@@ -1042,10 +1042,10 @@
     </row>
     <row r="59">
       <c r="A59" t="str">
-        <v>UniswapV3PoolSwapTest</v>
+        <v>IWETH</v>
       </c>
       <c r="B59">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C59">
         <v>0</v>
@@ -1053,10 +1053,10 @@
     </row>
     <row r="60">
       <c r="A60" t="str">
-        <v>UnsafeMathEchidnaTest</v>
+        <v>IndexesLens</v>
       </c>
       <c r="B60">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C60">
         <v>0</v>
@@ -1064,10 +1064,10 @@
     </row>
     <row r="61">
       <c r="A61" t="str">
-        <v>UniswapV3Factory</v>
+        <v>ILens</v>
       </c>
       <c r="B61">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C61">
         <v>0</v>
@@ -1075,10 +1075,10 @@
     </row>
     <row r="62">
       <c r="A62" t="str">
-        <v>UniswapV3Pool</v>
+        <v>Lens</v>
       </c>
       <c r="B62">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="C62">
         <v>0</v>
@@ -1086,18 +1086,172 @@
     </row>
     <row r="63">
       <c r="A63" t="str">
-        <v>UniswapV3PoolDeployer</v>
+        <v>LensStorage</v>
       </c>
       <c r="B63">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="C63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="str">
+        <v>MarketsLens</v>
+      </c>
+      <c r="B64">
+        <v>1</v>
+      </c>
+      <c r="C64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="str">
+        <v>RatesLens</v>
+      </c>
+      <c r="B65">
+        <v>1</v>
+      </c>
+      <c r="C65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="str">
+        <v>RewardsLens</v>
+      </c>
+      <c r="B66">
+        <v>1</v>
+      </c>
+      <c r="C66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="str">
+        <v>UsersLens</v>
+      </c>
+      <c r="B67">
+        <v>1</v>
+      </c>
+      <c r="C67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="str">
+        <v>CompoundMath</v>
+      </c>
+      <c r="B68">
+        <v>0</v>
+      </c>
+      <c r="C68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="str">
+        <v>InterestRatesModel</v>
+      </c>
+      <c r="B69">
+        <v>4</v>
+      </c>
+      <c r="C69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="str">
+        <v>Types</v>
+      </c>
+      <c r="B70">
+        <v>0</v>
+      </c>
+      <c r="C70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="str">
+        <v>MatchingEngine</v>
+      </c>
+      <c r="B71">
+        <v>1</v>
+      </c>
+      <c r="C71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="str">
+        <v>Morpho</v>
+      </c>
+      <c r="B72">
+        <v>1</v>
+      </c>
+      <c r="C72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="str">
+        <v>MorphoGovernance</v>
+      </c>
+      <c r="B73">
+        <v>1</v>
+      </c>
+      <c r="C73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="str">
+        <v>MorphoStorage</v>
+      </c>
+      <c r="B74">
+        <v>9</v>
+      </c>
+      <c r="C74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="str">
+        <v>MorphoUtils</v>
+      </c>
+      <c r="B75">
+        <v>5</v>
+      </c>
+      <c r="C75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="str">
+        <v>PositionsManager</v>
+      </c>
+      <c r="B76">
+        <v>3</v>
+      </c>
+      <c r="C76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="str">
+        <v>RewardsManager</v>
+      </c>
+      <c r="B77">
+        <v>4</v>
+      </c>
+      <c r="C77">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C63"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C77"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
code quality grades updated
</commit_message>
<xml_diff>
--- a/sheets/xlsxCouplings.xlsx
+++ b/sheets/xlsxCouplings.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C77"/>
+  <dimension ref="A1:C63"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -415,10 +415,10 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>EntryPositionsManager</v>
+        <v>IUniswapV3FlashCallback</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -426,10 +426,10 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>ExitPositionsManager</v>
+        <v>IUniswapV3MintCallback</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -437,10 +437,10 @@
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>IncentivesVault</v>
+        <v>IUniswapV3SwapCallback</v>
       </c>
       <c r="B4">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -448,10 +448,10 @@
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>InterestRatesManager</v>
+        <v>IERC20Minimal</v>
       </c>
       <c r="B5">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -459,7 +459,7 @@
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>IAaveDistributionManager</v>
+        <v>IUniswapV3Factory</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -470,10 +470,10 @@
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>IAaveIncentivesController</v>
+        <v>IUniswapV3Pool</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -481,10 +481,10 @@
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>IAToken</v>
+        <v>IUniswapV3PoolDeployer</v>
       </c>
       <c r="B8">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -492,7 +492,7 @@
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>IERC20</v>
+        <v>IUniswapV3PoolActions</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -503,10 +503,10 @@
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>ILendingPool</v>
+        <v>IUniswapV3PoolDerivedState</v>
       </c>
       <c r="B10">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -514,7 +514,7 @@
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>ILendingPoolAddressesProvider</v>
+        <v>IUniswapV3PoolEvents</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -525,7 +525,7 @@
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>IPriceOracleGetter</v>
+        <v>IUniswapV3PoolImmutables</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -536,7 +536,7 @@
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>IScaledBalanceToken</v>
+        <v>IUniswapV3PoolOwnerActions</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -547,10 +547,10 @@
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>IVariableDebtToken</v>
+        <v>IUniswapV3PoolState</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -558,7 +558,7 @@
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>IEntryPositionsManager</v>
+        <v>BitMath</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -569,7 +569,7 @@
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>IExitPositionsManager</v>
+        <v>FixedPoint128</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -580,7 +580,7 @@
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>IGetterUnderlyingAsset</v>
+        <v>FixedPoint96</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -591,10 +591,10 @@
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>IIncentivesVault</v>
+        <v>FullMath</v>
       </c>
       <c r="B18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -602,7 +602,7 @@
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>IInterestRatesManager</v>
+        <v>LiquidityMath</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -613,10 +613,10 @@
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>IMorpho</v>
+        <v>LowGasSafeMath</v>
       </c>
       <c r="B20">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C20">
         <v>0</v>
@@ -624,7 +624,7 @@
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>IOracle</v>
+        <v>Oracle</v>
       </c>
       <c r="B21">
         <v>0</v>
@@ -635,10 +635,10 @@
     </row>
     <row r="22">
       <c r="A22" t="str">
-        <v>IRewardsManager</v>
+        <v>Position</v>
       </c>
       <c r="B22">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C22">
         <v>0</v>
@@ -646,7 +646,7 @@
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v>ILido</v>
+        <v>SafeCast</v>
       </c>
       <c r="B23">
         <v>0</v>
@@ -657,10 +657,10 @@
     </row>
     <row r="24">
       <c r="A24" t="str">
-        <v>IndexesLens</v>
+        <v>SqrtPriceMath</v>
       </c>
       <c r="B24">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C24">
         <v>0</v>
@@ -668,10 +668,10 @@
     </row>
     <row r="25">
       <c r="A25" t="str">
-        <v>ILens</v>
+        <v>SwapMath</v>
       </c>
       <c r="B25">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C25">
         <v>0</v>
@@ -679,10 +679,10 @@
     </row>
     <row r="26">
       <c r="A26" t="str">
-        <v>Lens</v>
+        <v>Tick</v>
       </c>
       <c r="B26">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C26">
         <v>0</v>
@@ -690,10 +690,10 @@
     </row>
     <row r="27">
       <c r="A27" t="str">
-        <v>LensStorage</v>
+        <v>TickBitmap</v>
       </c>
       <c r="B27">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="C27">
         <v>0</v>
@@ -701,10 +701,10 @@
     </row>
     <row r="28">
       <c r="A28" t="str">
-        <v>MarketsLens</v>
+        <v>TickMath</v>
       </c>
       <c r="B28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C28">
         <v>0</v>
@@ -712,10 +712,10 @@
     </row>
     <row r="29">
       <c r="A29" t="str">
-        <v>RatesLens</v>
+        <v>TransferHelper</v>
       </c>
       <c r="B29">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C29">
         <v>0</v>
@@ -723,10 +723,10 @@
     </row>
     <row r="30">
       <c r="A30" t="str">
-        <v>UsersLens</v>
+        <v>UnsafeMath</v>
       </c>
       <c r="B30">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C30">
         <v>0</v>
@@ -734,7 +734,7 @@
     </row>
     <row r="31">
       <c r="A31" t="str">
-        <v>DataTypes</v>
+        <v>NoDelegateCall</v>
       </c>
       <c r="B31">
         <v>0</v>
@@ -745,10 +745,10 @@
     </row>
     <row r="32">
       <c r="A32" t="str">
-        <v>Errors</v>
+        <v>BitMathEchidnaTest</v>
       </c>
       <c r="B32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C32">
         <v>0</v>
@@ -756,10 +756,10 @@
     </row>
     <row r="33">
       <c r="A33" t="str">
-        <v>ReserveConfiguration</v>
+        <v>BitMathTest</v>
       </c>
       <c r="B33">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C33">
         <v>0</v>
@@ -767,7 +767,7 @@
     </row>
     <row r="34">
       <c r="A34" t="str">
-        <v>UserConfiguration</v>
+        <v>FullMathEchidnaTest</v>
       </c>
       <c r="B34">
         <v>1</v>
@@ -778,10 +778,10 @@
     </row>
     <row r="35">
       <c r="A35" t="str">
-        <v>InterestRatesModel</v>
+        <v>FullMathTest</v>
       </c>
       <c r="B35">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C35">
         <v>0</v>
@@ -789,10 +789,10 @@
     </row>
     <row r="36">
       <c r="A36" t="str">
-        <v>Types</v>
+        <v>LiquidityMathTest</v>
       </c>
       <c r="B36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C36">
         <v>0</v>
@@ -800,7 +800,7 @@
     </row>
     <row r="37">
       <c r="A37" t="str">
-        <v>MatchingEngine</v>
+        <v>LowGasSafeMathEchidnaTest</v>
       </c>
       <c r="B37">
         <v>1</v>
@@ -811,7 +811,7 @@
     </row>
     <row r="38">
       <c r="A38" t="str">
-        <v>Morpho</v>
+        <v>MockTimeUniswapV3Pool</v>
       </c>
       <c r="B38">
         <v>1</v>
@@ -822,7 +822,7 @@
     </row>
     <row r="39">
       <c r="A39" t="str">
-        <v>MorphoGovernance</v>
+        <v>MockTimeUniswapV3PoolDeployer</v>
       </c>
       <c r="B39">
         <v>2</v>
@@ -833,10 +833,10 @@
     </row>
     <row r="40">
       <c r="A40" t="str">
-        <v>MorphoStorage</v>
+        <v>NoDelegateCallTest</v>
       </c>
       <c r="B40">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C40">
         <v>0</v>
@@ -844,10 +844,10 @@
     </row>
     <row r="41">
       <c r="A41" t="str">
-        <v>MorphoUtils</v>
+        <v>OracleEchidnaTest</v>
       </c>
       <c r="B41">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C41">
         <v>0</v>
@@ -855,10 +855,10 @@
     </row>
     <row r="42">
       <c r="A42" t="str">
-        <v>PositionsManagerUtils</v>
+        <v>OracleTest</v>
       </c>
       <c r="B42">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C42">
         <v>0</v>
@@ -866,7 +866,7 @@
     </row>
     <row r="43">
       <c r="A43" t="str">
-        <v>RewardsDistributor</v>
+        <v>SqrtPriceMathEchidnaTest</v>
       </c>
       <c r="B43">
         <v>3</v>
@@ -877,7 +877,7 @@
     </row>
     <row r="44">
       <c r="A44" t="str">
-        <v>FakeToken</v>
+        <v>SqrtPriceMathTest</v>
       </c>
       <c r="B44">
         <v>1</v>
@@ -888,10 +888,10 @@
     </row>
     <row r="45">
       <c r="A45" t="str">
-        <v>IncentivesVault</v>
+        <v>SwapMathEchidnaTest</v>
       </c>
       <c r="B45">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C45">
         <v>0</v>
@@ -899,10 +899,10 @@
     </row>
     <row r="46">
       <c r="A46" t="str">
-        <v>InterestRatesManager</v>
+        <v>SwapMathTest</v>
       </c>
       <c r="B46">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C46">
         <v>0</v>
@@ -910,10 +910,10 @@
     </row>
     <row r="47">
       <c r="A47" t="str">
-        <v>ICEth</v>
+        <v>TestERC20</v>
       </c>
       <c r="B47">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C47">
         <v>0</v>
@@ -921,10 +921,10 @@
     </row>
     <row r="48">
       <c r="A48" t="str">
-        <v>IComptroller</v>
+        <v>TestUniswapV3Callee</v>
       </c>
       <c r="B48">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="C48">
         <v>0</v>
@@ -932,10 +932,10 @@
     </row>
     <row r="49">
       <c r="A49" t="str">
-        <v>IInterestRateModel</v>
+        <v>TestUniswapV3ReentrantCallee</v>
       </c>
       <c r="B49">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C49">
         <v>0</v>
@@ -943,10 +943,10 @@
     </row>
     <row r="50">
       <c r="A50" t="str">
-        <v>ICToken</v>
+        <v>TestUniswapV3Router</v>
       </c>
       <c r="B50">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C50">
         <v>0</v>
@@ -954,10 +954,10 @@
     </row>
     <row r="51">
       <c r="A51" t="str">
-        <v>ICEther</v>
+        <v>TestUniswapV3SwapPay</v>
       </c>
       <c r="B51">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C51">
         <v>0</v>
@@ -965,10 +965,10 @@
     </row>
     <row r="52">
       <c r="A52" t="str">
-        <v>ICompoundOracle</v>
+        <v>TickBitmapEchidnaTest</v>
       </c>
       <c r="B52">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C52">
         <v>0</v>
@@ -976,7 +976,7 @@
     </row>
     <row r="53">
       <c r="A53" t="str">
-        <v>IIncentivesVault</v>
+        <v>TickBitmapTest</v>
       </c>
       <c r="B53">
         <v>1</v>
@@ -987,10 +987,10 @@
     </row>
     <row r="54">
       <c r="A54" t="str">
-        <v>IInterestRatesManager</v>
+        <v>TickEchidnaTest</v>
       </c>
       <c r="B54">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C54">
         <v>0</v>
@@ -998,10 +998,10 @@
     </row>
     <row r="55">
       <c r="A55" t="str">
-        <v>IMorpho</v>
+        <v>TickMathEchidnaTest</v>
       </c>
       <c r="B55">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C55">
         <v>0</v>
@@ -1009,10 +1009,10 @@
     </row>
     <row r="56">
       <c r="A56" t="str">
-        <v>IOracle</v>
+        <v>TickMathTest</v>
       </c>
       <c r="B56">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C56">
         <v>0</v>
@@ -1020,10 +1020,10 @@
     </row>
     <row r="57">
       <c r="A57" t="str">
-        <v>IPositionsManager</v>
+        <v>TickOverflowSafetyEchidnaTest</v>
       </c>
       <c r="B57">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C57">
         <v>0</v>
@@ -1031,7 +1031,7 @@
     </row>
     <row r="58">
       <c r="A58" t="str">
-        <v>IRewardsManager</v>
+        <v>TickTest</v>
       </c>
       <c r="B58">
         <v>1</v>
@@ -1042,10 +1042,10 @@
     </row>
     <row r="59">
       <c r="A59" t="str">
-        <v>IWETH</v>
+        <v>UniswapV3PoolSwapTest</v>
       </c>
       <c r="B59">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C59">
         <v>0</v>
@@ -1053,10 +1053,10 @@
     </row>
     <row r="60">
       <c r="A60" t="str">
-        <v>IndexesLens</v>
+        <v>UnsafeMathEchidnaTest</v>
       </c>
       <c r="B60">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C60">
         <v>0</v>
@@ -1064,10 +1064,10 @@
     </row>
     <row r="61">
       <c r="A61" t="str">
-        <v>ILens</v>
+        <v>UniswapV3Factory</v>
       </c>
       <c r="B61">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C61">
         <v>0</v>
@@ -1075,10 +1075,10 @@
     </row>
     <row r="62">
       <c r="A62" t="str">
-        <v>Lens</v>
+        <v>UniswapV3Pool</v>
       </c>
       <c r="B62">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="C62">
         <v>0</v>
@@ -1086,172 +1086,18 @@
     </row>
     <row r="63">
       <c r="A63" t="str">
-        <v>LensStorage</v>
+        <v>UniswapV3PoolDeployer</v>
       </c>
       <c r="B63">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C63">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" t="str">
-        <v>MarketsLens</v>
-      </c>
-      <c r="B64">
-        <v>1</v>
-      </c>
-      <c r="C64">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" t="str">
-        <v>RatesLens</v>
-      </c>
-      <c r="B65">
-        <v>1</v>
-      </c>
-      <c r="C65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" t="str">
-        <v>RewardsLens</v>
-      </c>
-      <c r="B66">
-        <v>1</v>
-      </c>
-      <c r="C66">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" t="str">
-        <v>UsersLens</v>
-      </c>
-      <c r="B67">
-        <v>1</v>
-      </c>
-      <c r="C67">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" t="str">
-        <v>CompoundMath</v>
-      </c>
-      <c r="B68">
-        <v>0</v>
-      </c>
-      <c r="C68">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" t="str">
-        <v>InterestRatesModel</v>
-      </c>
-      <c r="B69">
-        <v>4</v>
-      </c>
-      <c r="C69">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" t="str">
-        <v>Types</v>
-      </c>
-      <c r="B70">
-        <v>0</v>
-      </c>
-      <c r="C70">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" t="str">
-        <v>MatchingEngine</v>
-      </c>
-      <c r="B71">
-        <v>1</v>
-      </c>
-      <c r="C71">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" t="str">
-        <v>Morpho</v>
-      </c>
-      <c r="B72">
-        <v>1</v>
-      </c>
-      <c r="C72">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" t="str">
-        <v>MorphoGovernance</v>
-      </c>
-      <c r="B73">
-        <v>1</v>
-      </c>
-      <c r="C73">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" t="str">
-        <v>MorphoStorage</v>
-      </c>
-      <c r="B74">
-        <v>9</v>
-      </c>
-      <c r="C74">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" t="str">
-        <v>MorphoUtils</v>
-      </c>
-      <c r="B75">
-        <v>5</v>
-      </c>
-      <c r="C75">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" t="str">
-        <v>PositionsManager</v>
-      </c>
-      <c r="B76">
-        <v>3</v>
-      </c>
-      <c r="C76">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" t="str">
-        <v>RewardsManager</v>
-      </c>
-      <c r="B77">
-        <v>4</v>
-      </c>
-      <c r="C77">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C77"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C63"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>